<commit_message>
Other procedures add in
</commit_message>
<xml_diff>
--- a/Mapping/Other Packages.xlsx
+++ b/Mapping/Other Packages.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Array Types" sheetId="7" r:id="rId4"/>
     <sheet name="Constants" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Group</t>
   </si>
@@ -107,6 +107,33 @@
   </si>
   <si>
     <t>Setups all of the variables for the engage run</t>
+  </si>
+  <si>
+    <t>Index Type</t>
+  </si>
+  <si>
+    <t>Array Values Type</t>
+  </si>
+  <si>
+    <t>General_Checks</t>
+  </si>
+  <si>
+    <t>Mask_Type</t>
+  </si>
+  <si>
+    <t>Mask_Index_Array_Type</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Constant Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Attribute</t>
   </si>
 </sst>
 </file>
@@ -459,7 +486,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +591,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,10 +658,10 @@
         <v>24</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -716,26 +743,88 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change of direction in failure thought ou
</commit_message>
<xml_diff>
--- a/Mapping/Other Packages.xlsx
+++ b/Mapping/Other Packages.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Group</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Initialise_Engager</t>
   </si>
   <si>
-    <t>Setups all of the variables for the engage run</t>
-  </si>
-  <si>
     <t>Index Type</t>
   </si>
   <si>
@@ -134,6 +131,39 @@
   </si>
   <si>
     <t>Attribute</t>
+  </si>
+  <si>
+    <t>Setups the variables for the engage run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While Check_Value &lt; 5
+       Increment Check_Value + 1
+       If Check_Value = 2
+             Set Ex_Range_Distance_1 
+             Ex_Range_Distance_2 to max
+       If Check_Value = 3
+             Set Ex_Range_Distance_1 
+             Ex_Range_Distance_2 to min
+</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Call_Failure</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Input a test Id to see if a failure occurred</t>
+  </si>
+  <si>
+    <t>Test_Id Local = Test_Id
+If Failure_Data_Structure(Tests_Id_Local) = True</t>
+  </si>
+  <si>
+    <t>Hex_Value_Lock</t>
   </si>
 </sst>
 </file>
@@ -486,7 +516,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +525,7 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -519,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -530,14 +560,28 @@
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="3"/>
@@ -591,7 +635,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,24 +809,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -792,17 +836,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -812,16 +856,33 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>